<commit_message>
Example Added - post message to Kafka topic
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/CreateOrder-Event.xlsx
+++ b/rest-db-kafka/src/test/resources/CreateOrder-Event.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93D8CF-26E2-4EC9-8158-BC669FE38279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1215F323-0669-4AFC-AB0D-0600CAED928F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderCreated-Event" sheetId="1" r:id="rId1"/>
+    <sheet name="PostMessage-Event" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -151,6 +152,38 @@
   </si>
   <si>
     <t>JSONType</t>
+  </si>
+  <si>
+    <t>SendOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @simple-send</t>
+  </si>
+  <si>
+    <t>{
+  "customer": {
+    "customerId": 1001,
+    "firstname": "Ronnie",
+    "lastname": "Sander"
+  },
+  "orderNumber" : "1234-1234-1234",
+  "orderDesc": "Order Dell Laptop",
+  "orderStatus": "Started",
+  "purchasedProducts": [
+    {
+      "productId": 901,
+      "productName": "Dell Inspiron 3583 15",
+      "productDesc": "Laptop Intel Celeron – 128GB SSD – 4GB DDR4 – 1.6GHz - Intel UHD Graphics 610 - Windows 10 Home in S Mode - Inspiron 15 3000 Series"
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>1234-1234-1234</t>
+  </si>
+  <si>
+    <t>orderNumber,orderDesc,orderStatus, customer/customerId:firstname:lastname,orderStatus
+1234-1234-1234,Order Dell Laptop,Started,i~1001:Ronnie:Sander,Started</t>
   </si>
 </sst>
 </file>
@@ -474,29 +507,29 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.27734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.1640625" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="85.71875" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="85.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="85.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="85.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="265.2" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:16" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -590,7 +623,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -637,4 +670,152 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B8F9F1-284E-4A03-9CF1-DA17E9F6F966}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="72.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="91" customWidth="1"/>
+    <col min="15" max="15" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>